<commit_message>
Fixed some display settings
</commit_message>
<xml_diff>
--- a/data/personality traits builder.xlsx
+++ b/data/personality traits builder.xlsx
@@ -342,7 +342,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="11">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -360,66 +360,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -458,15 +398,9 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:Q78" totalsRowShown="0">
-  <autoFilter ref="A2:Q78">
-    <filterColumn colId="6">
-      <customFilters>
-        <customFilter operator="notEqual" val="0"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:Q78"/>
   <sortState ref="A3:Q78">
-    <sortCondition ref="G2:G78"/>
+    <sortCondition ref="A2:A78"/>
   </sortState>
   <tableColumns count="17">
     <tableColumn id="1" name="Name"/>
@@ -478,16 +412,16 @@
     <tableColumn id="7" name="Total">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="unique name" dataDxfId="15">
+    <tableColumn id="8" name="unique name" dataDxfId="9">
       <calculatedColumnFormula array="1">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="string values" dataDxfId="14">
+    <tableColumn id="9" name="string values" dataDxfId="8">
       <calculatedColumnFormula>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="unique values" dataDxfId="12">
+    <tableColumn id="10" name="unique values" dataDxfId="7">
       <calculatedColumnFormula array="1">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Unique?" dataDxfId="13">
+    <tableColumn id="11" name="Unique?" dataDxfId="6">
       <calculatedColumnFormula array="1">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" name="Column1" dataDxfId="5">
@@ -780,7 +714,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D82" sqref="D82"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,7 +723,7 @@
     <col min="2" max="7" width="16.140625" customWidth="1"/>
     <col min="8" max="10" width="16.140625" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="10.5703125" customWidth="1"/>
-    <col min="12" max="16" width="16.140625" customWidth="1"/>
+    <col min="12" max="16" width="16.140625" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="94.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -874,20 +808,20 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3">
-        <v>-3</v>
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
       </c>
       <c r="D3">
-        <v>-3</v>
-      </c>
-      <c r="E3">
+        <v>-4</v>
+      </c>
+      <c r="F3">
         <v>2</v>
       </c>
       <c r="G3">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>-4</v>
+        <v>2</v>
       </c>
       <c r="H3">
         <f t="array" ref="H3">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -895,7 +829,7 @@
       </c>
       <c r="I3" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>-30-320</v>
+        <v>04-402</v>
       </c>
       <c r="J3">
         <f t="array" ref="J3">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
@@ -907,45 +841,45 @@
       </c>
       <c r="L3" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
-        <v xml:space="preserve">"determination": -3, </v>
+        <v/>
       </c>
       <c r="M3" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"enthusiasm": 4, </v>
       </c>
       <c r="N3" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v xml:space="preserve">"stability": -3, </v>
+        <v xml:space="preserve">"stability": -4, </v>
       </c>
       <c r="O3" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
-        <v xml:space="preserve">"insight": 2, </v>
+        <v/>
       </c>
       <c r="P3" t="str">
         <f>IF(Table1[[#This Row],[Mysticism]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Mysticism]]) &amp; """: " &amp; Table1[[#This Row],[Mysticism]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"mysticism": 2, </v>
       </c>
       <c r="Q3" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "annoyed": {"determination": -3, "stability": -3, "insight": 2, },</v>
+        <v xml:space="preserve">    "adventurous": {"enthusiasm": 4, "stability": -4, "mysticism": 2, },</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>-2</v>
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>-3</v>
       </c>
       <c r="E4">
-        <v>-2</v>
+        <v>4</v>
       </c>
       <c r="G4">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>-2</v>
+        <v>5</v>
       </c>
       <c r="H4">
         <f t="array" ref="H4">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -953,7 +887,7 @@
       </c>
       <c r="I4" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>20-2-20</v>
+        <v>4-3040</v>
       </c>
       <c r="J4">
         <f t="array" ref="J4">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
@@ -965,19 +899,19 @@
       </c>
       <c r="L4" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
-        <v xml:space="preserve">"determination": 2, </v>
+        <v xml:space="preserve">"determination": 4, </v>
       </c>
       <c r="M4" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"enthusiasm": -3, </v>
       </c>
       <c r="N4" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v xml:space="preserve">"stability": -2, </v>
+        <v/>
       </c>
       <c r="O4" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
-        <v xml:space="preserve">"insight": -2, </v>
+        <v xml:space="preserve">"insight": 4, </v>
       </c>
       <c r="P4" t="str">
         <f>IF(Table1[[#This Row],[Mysticism]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Mysticism]]) &amp; """: " &amp; Table1[[#This Row],[Mysticism]] &amp; ", ")</f>
@@ -985,28 +919,25 @@
       </c>
       <c r="Q4" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "bossy": {"determination": 2, "stability": -2, "insight": -2, },</v>
+        <v xml:space="preserve">    "ambitious": {"determination": 4, "enthusiasm": -3, "insight": 4, },</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="B5">
-        <v>-5</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
+        <v>-3</v>
       </c>
       <c r="D5">
+        <v>-3</v>
+      </c>
+      <c r="E5">
         <v>2</v>
       </c>
-      <c r="E5">
-        <v>-3</v>
-      </c>
       <c r="G5">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="H5">
         <f t="array" ref="H5">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -1014,7 +945,7 @@
       </c>
       <c r="I5" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>-552-30</v>
+        <v>-30-320</v>
       </c>
       <c r="J5">
         <f t="array" ref="J5">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
@@ -1026,19 +957,19 @@
       </c>
       <c r="L5" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
-        <v xml:space="preserve">"determination": -5, </v>
+        <v xml:space="preserve">"determination": -3, </v>
       </c>
       <c r="M5" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
-        <v xml:space="preserve">"enthusiasm": 5, </v>
+        <v/>
       </c>
       <c r="N5" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v xml:space="preserve">"stability": 2, </v>
+        <v xml:space="preserve">"stability": -3, </v>
       </c>
       <c r="O5" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
-        <v xml:space="preserve">"insight": -3, </v>
+        <v xml:space="preserve">"insight": 2, </v>
       </c>
       <c r="P5" t="str">
         <f>IF(Table1[[#This Row],[Mysticism]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Mysticism]]) &amp; """: " &amp; Table1[[#This Row],[Mysticism]] &amp; ", ")</f>
@@ -1046,16 +977,25 @@
       </c>
       <c r="Q5" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "carefree": {"determination": -5, "enthusiasm": 5, "stability": 2, "insight": -3, },</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "annoyed": {"determination": -3, "stability": -3, "insight": 2, },</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>-2</v>
+      </c>
+      <c r="E6">
+        <v>-2</v>
       </c>
       <c r="G6">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="H6">
         <f t="array" ref="H6">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -1063,19 +1003,19 @@
       </c>
       <c r="I6" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00000</v>
+        <v>20-2-20</v>
       </c>
       <c r="J6">
         <f t="array" ref="J6">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="K6" t="b">
         <f t="array" ref="K6">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"determination": 2, </v>
       </c>
       <c r="M6" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
@@ -1083,11 +1023,11 @@
       </c>
       <c r="N6" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"stability": -2, </v>
       </c>
       <c r="O6" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"insight": -2, </v>
       </c>
       <c r="P6" t="str">
         <f>IF(Table1[[#This Row],[Mysticism]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Mysticism]]) &amp; """: " &amp; Table1[[#This Row],[Mysticism]] &amp; ", ")</f>
@@ -1095,16 +1035,25 @@
       </c>
       <c r="Q6" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "conceited": {},</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "bossy": {"determination": 2, "stability": -2, "insight": -2, },</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>-2</v>
       </c>
       <c r="G7">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H7">
         <f t="array" ref="H7">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -1112,23 +1061,23 @@
       </c>
       <c r="I7" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00000</v>
+        <v>520-20</v>
       </c>
       <c r="J7">
         <f t="array" ref="J7">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="K7" t="b">
         <f t="array" ref="K7">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"determination": 5, </v>
       </c>
       <c r="M7" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"enthusiasm": 2, </v>
       </c>
       <c r="N7" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
@@ -1136,7 +1085,7 @@
       </c>
       <c r="O7" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"insight": -2, </v>
       </c>
       <c r="P7" t="str">
         <f>IF(Table1[[#This Row],[Mysticism]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Mysticism]]) &amp; """: " &amp; Table1[[#This Row],[Mysticism]] &amp; ", ")</f>
@@ -1144,16 +1093,25 @@
       </c>
       <c r="Q7" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "considerate": {},</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "brave": {"determination": 5, "enthusiasm": 2, "insight": -2, },</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <v>-2</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
       </c>
       <c r="G8">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H8">
         <f t="array" ref="H8">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -1161,15 +1119,15 @@
       </c>
       <c r="I8" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00000</v>
+        <v>00-262</v>
       </c>
       <c r="J8">
         <f t="array" ref="J8">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="K8" t="b">
         <f t="array" ref="K8">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
@@ -1181,28 +1139,34 @@
       </c>
       <c r="N8" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"stability": -2, </v>
       </c>
       <c r="O8" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"insight": 6, </v>
       </c>
       <c r="P8" t="str">
         <f>IF(Table1[[#This Row],[Mysticism]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Mysticism]]) &amp; """: " &amp; Table1[[#This Row],[Mysticism]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"mysticism": 2, </v>
       </c>
       <c r="Q8" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "cooperative": {},</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "brilliant": {"stability": -2, "insight": 6, "mysticism": 2, },</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>52</v>
+      </c>
+      <c r="C9">
+        <v>-4</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
       </c>
       <c r="G9">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H9">
         <f t="array" ref="H9">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -1210,15 +1174,15 @@
       </c>
       <c r="I9" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00000</v>
+        <v>0-4600</v>
       </c>
       <c r="J9">
         <f t="array" ref="J9">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="K9" t="b">
         <f t="array" ref="K9">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
@@ -1226,11 +1190,11 @@
       </c>
       <c r="M9" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"enthusiasm": -4, </v>
       </c>
       <c r="N9" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"stability": 6, </v>
       </c>
       <c r="O9" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
@@ -1242,16 +1206,28 @@
       </c>
       <c r="Q9" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "curious": {},</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "calm": {"enthusiasm": -4, "stability": 6, },</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>-5</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>-3</v>
       </c>
       <c r="G10">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H10">
         <f t="array" ref="H10">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -1259,31 +1235,31 @@
       </c>
       <c r="I10" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00000</v>
+        <v>-552-30</v>
       </c>
       <c r="J10">
         <f t="array" ref="J10">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="K10" t="b">
         <f t="array" ref="K10">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"determination": -5, </v>
       </c>
       <c r="M10" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"enthusiasm": 5, </v>
       </c>
       <c r="N10" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"stability": 2, </v>
       </c>
       <c r="O10" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"insight": -3, </v>
       </c>
       <c r="P10" t="str">
         <f>IF(Table1[[#This Row],[Mysticism]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Mysticism]]) &amp; """: " &amp; Table1[[#This Row],[Mysticism]] &amp; ", ")</f>
@@ -1291,16 +1267,28 @@
       </c>
       <c r="Q10" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "demanding": {},</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "carefree": {"determination": -5, "enthusiasm": 5, "stability": 2, "insight": -3, },</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>33</v>
+      </c>
+      <c r="C11">
+        <v>-4</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>-3</v>
       </c>
       <c r="G11">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H11">
         <f t="array" ref="H11">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -1308,15 +1296,15 @@
       </c>
       <c r="I11" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00000</v>
+        <v>0-446-3</v>
       </c>
       <c r="J11">
         <f t="array" ref="J11">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="K11" t="b">
         <f t="array" ref="K11">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
@@ -1324,32 +1312,41 @@
       </c>
       <c r="M11" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"enthusiasm": -4, </v>
       </c>
       <c r="N11" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"stability": 4, </v>
       </c>
       <c r="O11" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"insight": 6, </v>
       </c>
       <c r="P11" t="str">
         <f>IF(Table1[[#This Row],[Mysticism]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Mysticism]]) &amp; """: " &amp; Table1[[#This Row],[Mysticism]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"mysticism": -3, </v>
       </c>
       <c r="Q11" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "eager": {},</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "cautious": {"enthusiasm": -4, "stability": 4, "insight": 6, "mysticism": -3, },</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>29</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>-2</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
       </c>
       <c r="G12">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H12">
         <f t="array" ref="H12">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -1357,19 +1354,19 @@
       </c>
       <c r="I12" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00000</v>
+        <v>200-22</v>
       </c>
       <c r="J12">
         <f t="array" ref="J12">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="K12" t="b">
         <f t="array" ref="K12">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"determination": 2, </v>
       </c>
       <c r="M12" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
@@ -1381,20 +1378,20 @@
       </c>
       <c r="O12" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"insight": -2, </v>
       </c>
       <c r="P12" t="str">
         <f>IF(Table1[[#This Row],[Mysticism]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Mysticism]]) &amp; """: " &amp; Table1[[#This Row],[Mysticism]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"mysticism": 2, </v>
       </c>
       <c r="Q12" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "faithful": {},</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "charming": {"determination": 2, "insight": -2, "mysticism": 2, },</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="G13">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -1438,12 +1435,12 @@
       </c>
       <c r="Q13" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "foolish": {},</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "conceited": {},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G14">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -1487,12 +1484,12 @@
       </c>
       <c r="Q14" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "generous": {},</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "considerate": {},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="G15">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -1536,16 +1533,25 @@
       </c>
       <c r="Q15" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "gentle": {},</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "cooperative": {},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>19</v>
+      </c>
+      <c r="D16">
+        <v>-2</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>6</v>
       </c>
       <c r="G16">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H16">
         <f t="array" ref="H16">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -1553,15 +1559,15 @@
       </c>
       <c r="I16" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00000</v>
+        <v>00-226</v>
       </c>
       <c r="J16">
         <f t="array" ref="J16">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="K16" t="b">
         <f t="array" ref="K16">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
@@ -1573,24 +1579,24 @@
       </c>
       <c r="N16" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"stability": -2, </v>
       </c>
       <c r="O16" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"insight": 2, </v>
       </c>
       <c r="P16" t="str">
         <f>IF(Table1[[#This Row],[Mysticism]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Mysticism]]) &amp; """: " &amp; Table1[[#This Row],[Mysticism]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"mysticism": 6, </v>
       </c>
       <c r="Q16" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "grumpy": {},</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "creative": {"stability": -2, "insight": 2, "mysticism": 6, },</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="G17">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -1634,16 +1640,28 @@
       </c>
       <c r="Q17" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "gullible": {},</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "curious": {},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>-4</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
       </c>
       <c r="G18">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18">
         <f t="array" ref="H18">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -1651,19 +1669,19 @@
       </c>
       <c r="I18" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00000</v>
+        <v>202-42</v>
       </c>
       <c r="J18">
         <f t="array" ref="J18">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="K18" t="b">
         <f t="array" ref="K18">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"determination": 2, </v>
       </c>
       <c r="M18" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
@@ -1671,24 +1689,24 @@
       </c>
       <c r="N18" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"stability": 2, </v>
       </c>
       <c r="O18" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"insight": -4, </v>
       </c>
       <c r="P18" t="str">
         <f>IF(Table1[[#This Row],[Mysticism]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Mysticism]]) &amp; """: " &amp; Table1[[#This Row],[Mysticism]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"mysticism": 2, </v>
       </c>
       <c r="Q18" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "hardworking": {},</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "daring": {"determination": 2, "stability": 2, "insight": -4, "mysticism": 2, },</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G19">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -1732,16 +1750,25 @@
       </c>
       <c r="Q19" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "helpful": {},</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "demanding": {},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>50</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>-2</v>
+      </c>
+      <c r="F20">
+        <v>-2</v>
       </c>
       <c r="G20">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H20">
         <f t="array" ref="H20">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -1749,23 +1776,23 @@
       </c>
       <c r="I20" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00000</v>
+        <v>6-200-2</v>
       </c>
       <c r="J20">
         <f t="array" ref="J20">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="K20" t="b">
         <f t="array" ref="K20">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"determination": 6, </v>
       </c>
       <c r="M20" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"enthusiasm": -2, </v>
       </c>
       <c r="N20" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
@@ -1777,16 +1804,16 @@
       </c>
       <c r="P20" t="str">
         <f>IF(Table1[[#This Row],[Mysticism]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Mysticism]]) &amp; """: " &amp; Table1[[#This Row],[Mysticism]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"mysticism": -2, </v>
       </c>
       <c r="Q20" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "honest": {},</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "determined": {"determination": 6, "enthusiasm": -2, "mysticism": -2, },</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="G21">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -1830,16 +1857,22 @@
       </c>
       <c r="Q21" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "imaginative": {},</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "eager": {},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>51</v>
+      </c>
+      <c r="C22">
+        <v>6</v>
+      </c>
+      <c r="D22">
+        <v>-2</v>
       </c>
       <c r="G22">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H22">
         <f t="array" ref="H22">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -1847,15 +1880,15 @@
       </c>
       <c r="I22" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00000</v>
+        <v>06-200</v>
       </c>
       <c r="J22">
         <f t="array" ref="J22">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="K22" t="b">
         <f t="array" ref="K22">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
@@ -1863,11 +1896,11 @@
       </c>
       <c r="M22" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"enthusiasm": 6, </v>
       </c>
       <c r="N22" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"stability": -2, </v>
       </c>
       <c r="O22" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
@@ -1879,12 +1912,12 @@
       </c>
       <c r="Q22" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "independent": {},</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "energetic": {"enthusiasm": 6, "stability": -2, },</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="G23">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -1928,12 +1961,12 @@
       </c>
       <c r="Q23" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "intelligent": {},</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "faithful": {},</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="G24">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -1977,12 +2010,12 @@
       </c>
       <c r="Q24" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "jealous": {},</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "foolish": {},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="G25">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -2026,30 +2059,30 @@
       </c>
       <c r="Q25" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "lazy": {},</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "generous": {},</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>90</v>
+        <v>38</v>
       </c>
       <c r="G26">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
         <v>0</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H26">
         <f t="array" ref="H26">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
         <v>1</v>
       </c>
-      <c r="I26" s="1" t="str">
-        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00000</v>
-      </c>
-      <c r="J26" s="1">
+      <c r="I26" t="str">
+        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
+        <v>00000</v>
+      </c>
+      <c r="J26">
         <f t="array" ref="J26">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
         <v>59</v>
       </c>
-      <c r="K26" s="1" t="b">
+      <c r="K26" t="b">
         <f t="array" ref="K26">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
         <v>0</v>
       </c>
@@ -2075,12 +2108,12 @@
       </c>
       <c r="Q26" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "lively": {},</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "gentle": {},</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="G27">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -2124,12 +2157,12 @@
       </c>
       <c r="Q27" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "lonely": {},</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "grumpy": {},</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G28">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -2173,12 +2206,12 @@
       </c>
       <c r="Q28" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "loyal": {},</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "gullible": {},</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="G29">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -2222,12 +2255,12 @@
       </c>
       <c r="Q29" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "lucky": {},</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "hardworking": {},</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="G30">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -2271,12 +2304,12 @@
       </c>
       <c r="Q30" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "mannerly": {},</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "helpful": {},</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="G31">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -2320,16 +2353,25 @@
       </c>
       <c r="Q31" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "mature": {},</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "honest": {},</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>42</v>
+      </c>
+      <c r="B32">
+        <v>-2</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
       </c>
       <c r="G32">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H32">
         <f t="array" ref="H32">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -2337,27 +2379,27 @@
       </c>
       <c r="I32" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00000</v>
+        <v>-24200</v>
       </c>
       <c r="J32">
         <f t="array" ref="J32">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="K32" t="b">
         <f t="array" ref="K32">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L32" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"determination": -2, </v>
       </c>
       <c r="M32" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"enthusiasm": 4, </v>
       </c>
       <c r="N32" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"stability": 2, </v>
       </c>
       <c r="O32" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
@@ -2369,16 +2411,25 @@
       </c>
       <c r="Q32" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "mischievous": {},</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "hopeful": {"determination": -2, "enthusiasm": 4, "stability": 2, },</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>-2</v>
+      </c>
+      <c r="C33">
+        <v>-1</v>
+      </c>
+      <c r="D33">
+        <v>6</v>
       </c>
       <c r="G33">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H33">
         <f t="array" ref="H33">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -2386,27 +2437,27 @@
       </c>
       <c r="I33" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00000</v>
+        <v>-2-1600</v>
       </c>
       <c r="J33">
         <f t="array" ref="J33">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="K33" t="b">
         <f t="array" ref="K33">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L33" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"determination": -2, </v>
       </c>
       <c r="M33" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"enthusiasm": -1, </v>
       </c>
       <c r="N33" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"stability": 6, </v>
       </c>
       <c r="O33" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
@@ -2418,12 +2469,12 @@
       </c>
       <c r="Q33" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "miserable": {},</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "humble": {"determination": -2, "enthusiasm": -1, "stability": 6, },</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="G34">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -2467,30 +2518,30 @@
       </c>
       <c r="Q34" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "mysterious": {},</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "imaginative": {},</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>88</v>
+        <v>20</v>
       </c>
       <c r="G35">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
         <v>0</v>
       </c>
-      <c r="H35" s="1">
+      <c r="H35">
         <f t="array" ref="H35">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
         <v>1</v>
       </c>
-      <c r="I35" s="1" t="str">
-        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00000</v>
-      </c>
-      <c r="J35" s="1">
+      <c r="I35" t="str">
+        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
+        <v>00000</v>
+      </c>
+      <c r="J35">
         <f t="array" ref="J35">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
         <v>59</v>
       </c>
-      <c r="K35" s="1" t="b">
+      <c r="K35" t="b">
         <f t="array" ref="K35">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
         <v>0</v>
       </c>
@@ -2516,12 +2567,12 @@
       </c>
       <c r="Q35" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "opaque": {},</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "independent": {},</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="G36">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -2565,12 +2616,12 @@
       </c>
       <c r="Q36" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "polite": {},</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "intelligent": {},</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="G37">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -2614,12 +2665,12 @@
       </c>
       <c r="Q37" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "proud": {},</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "jealous": {},</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="G38">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -2663,30 +2714,30 @@
       </c>
       <c r="Q38" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "quiet": {},</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "lazy": {},</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="G39">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
         <v>0</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="1">
         <f t="array" ref="H39">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
         <v>1</v>
       </c>
-      <c r="I39" t="str">
-        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00000</v>
-      </c>
-      <c r="J39">
+      <c r="I39" s="1" t="str">
+        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
+        <v>00000</v>
+      </c>
+      <c r="J39" s="1">
         <f t="array" ref="J39">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
         <v>59</v>
       </c>
-      <c r="K39" t="b">
+      <c r="K39" s="1" t="b">
         <f t="array" ref="K39">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
         <v>0</v>
       </c>
@@ -2712,12 +2763,12 @@
       </c>
       <c r="Q39" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "rad": {},</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "lively": {},</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="G40">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -2761,12 +2812,12 @@
       </c>
       <c r="Q40" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "resourceful": {},</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "lonely": {},</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G41">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -2810,12 +2861,12 @@
       </c>
       <c r="Q41" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "respectful": {},</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "loyal": {},</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G42">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -2859,12 +2910,12 @@
       </c>
       <c r="Q42" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "responsible": {},</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "lucky": {},</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="G43">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -2908,12 +2959,12 @@
       </c>
       <c r="Q43" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "rich": {},</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "mannerly": {},</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G44">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -2957,12 +3008,12 @@
       </c>
       <c r="Q44" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "rude": {},</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "mature": {},</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G45">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -3006,12 +3057,12 @@
       </c>
       <c r="Q45" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "self-confident": {},</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "mischievous": {},</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="G46">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -3055,30 +3106,30 @@
       </c>
       <c r="Q46" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "selfish": {},</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "miserable": {},</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="G47">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
         <v>0</v>
       </c>
-      <c r="H47" s="1">
+      <c r="H47">
         <f t="array" ref="H47">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
         <v>1</v>
       </c>
-      <c r="I47" s="1" t="str">
-        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00000</v>
-      </c>
-      <c r="J47" s="1">
+      <c r="I47" t="str">
+        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
+        <v>00000</v>
+      </c>
+      <c r="J47">
         <f t="array" ref="J47">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
         <v>59</v>
       </c>
-      <c r="K47" s="1" t="b">
+      <c r="K47" t="b">
         <f t="array" ref="K47">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
         <v>0</v>
       </c>
@@ -3104,30 +3155,30 @@
       </c>
       <c r="Q47" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "shining": {},</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "mysterious": {},</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="G48">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
         <v>0</v>
       </c>
-      <c r="H48">
+      <c r="H48" s="1">
         <f t="array" ref="H48">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
         <v>1</v>
       </c>
-      <c r="I48" t="str">
-        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00000</v>
-      </c>
-      <c r="J48">
+      <c r="I48" s="1" t="str">
+        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
+        <v>00000</v>
+      </c>
+      <c r="J48" s="1">
         <f t="array" ref="J48">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
         <v>59</v>
       </c>
-      <c r="K48" t="b">
+      <c r="K48" s="1" t="b">
         <f t="array" ref="K48">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
         <v>0</v>
       </c>
@@ -3153,12 +3204,12 @@
       </c>
       <c r="Q48" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "shy": {},</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "opaque": {},</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="G49">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -3202,12 +3253,12 @@
       </c>
       <c r="Q49" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "skillful": {},</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "polite": {},</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="G50">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -3251,12 +3302,12 @@
       </c>
       <c r="Q50" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "sly": {},</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "proud": {},</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="G51">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -3300,12 +3351,12 @@
       </c>
       <c r="Q51" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "strict": {},</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "quiet": {},</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="G52">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -3349,12 +3400,12 @@
       </c>
       <c r="Q52" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "stubborn": {},</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "rad": {},</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="G53">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -3362,7 +3413,7 @@
       </c>
       <c r="H53">
         <f t="array" ref="H53">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I53" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
@@ -3398,30 +3449,30 @@
       </c>
       <c r="Q53" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "studious": {},</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "resourceful": {},</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G54">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
         <v>0</v>
       </c>
-      <c r="H54" s="1">
+      <c r="H54">
         <f t="array" ref="H54">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
-        <v>2</v>
-      </c>
-      <c r="I54" s="1" t="str">
-        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00000</v>
-      </c>
-      <c r="J54" s="1">
+        <v>1</v>
+      </c>
+      <c r="I54" t="str">
+        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
+        <v>00000</v>
+      </c>
+      <c r="J54">
         <f t="array" ref="J54">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
         <v>59</v>
       </c>
-      <c r="K54" s="1" t="b">
+      <c r="K54" t="b">
         <f t="array" ref="K54">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
         <v>0</v>
       </c>
@@ -3447,12 +3498,12 @@
       </c>
       <c r="Q54" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "studious": {},</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "respectful": {},</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="G55">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -3496,12 +3547,12 @@
       </c>
       <c r="Q55" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "talented": {},</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "responsible": {},</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G56">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -3545,12 +3596,12 @@
       </c>
       <c r="Q56" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "thoughtful": {},</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "rich": {},</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="G57">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -3594,30 +3645,30 @@
       </c>
       <c r="Q57" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "timid": {},</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "rude": {},</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>86</v>
+        <v>14</v>
       </c>
       <c r="G58">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
         <v>0</v>
       </c>
-      <c r="H58" s="1">
+      <c r="H58">
         <f t="array" ref="H58">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
         <v>1</v>
       </c>
-      <c r="I58" s="1" t="str">
-        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00000</v>
-      </c>
-      <c r="J58" s="1">
+      <c r="I58" t="str">
+        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
+        <v>00000</v>
+      </c>
+      <c r="J58">
         <f t="array" ref="J58">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
         <v>59</v>
       </c>
-      <c r="K58" s="1" t="b">
+      <c r="K58" t="b">
         <f t="array" ref="K58">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
         <v>0</v>
       </c>
@@ -3643,12 +3694,12 @@
       </c>
       <c r="Q58" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "tired": {},</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "self-confident": {},</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="G59">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -3692,16 +3743,28 @@
       </c>
       <c r="Q59" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "tolerant": {},</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "selfish": {},</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>66</v>
+        <v>7</v>
+      </c>
+      <c r="C60">
+        <v>-3</v>
+      </c>
+      <c r="D60">
+        <v>5</v>
+      </c>
+      <c r="E60">
+        <v>2</v>
+      </c>
+      <c r="F60">
+        <v>-3</v>
       </c>
       <c r="G60">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H60">
         <f t="array" ref="H60">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -3709,15 +3772,15 @@
       </c>
       <c r="I60" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00000</v>
+        <v>0-352-3</v>
       </c>
       <c r="J60">
         <f t="array" ref="J60">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="K60" t="b">
         <f t="array" ref="K60">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L60" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
@@ -3725,46 +3788,46 @@
       </c>
       <c r="M60" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"enthusiasm": -3, </v>
       </c>
       <c r="N60" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"stability": 5, </v>
       </c>
       <c r="O60" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"insight": 2, </v>
       </c>
       <c r="P60" t="str">
         <f>IF(Table1[[#This Row],[Mysticism]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Mysticism]]) &amp; """: " &amp; Table1[[#This Row],[Mysticism]] &amp; ", ")</f>
-        <v/>
+        <v xml:space="preserve">"mysticism": -3, </v>
       </c>
       <c r="Q60" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "trustworthy": {},</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "serious": {"enthusiasm": -3, "stability": 5, "insight": 2, "mysticism": -3, },</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="G61">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
         <v>0</v>
       </c>
-      <c r="H61">
+      <c r="H61" s="1">
         <f t="array" ref="H61">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
         <v>1</v>
       </c>
-      <c r="I61" t="str">
-        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00000</v>
-      </c>
-      <c r="J61">
+      <c r="I61" s="1" t="str">
+        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
+        <v>00000</v>
+      </c>
+      <c r="J61" s="1">
         <f t="array" ref="J61">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
         <v>59</v>
       </c>
-      <c r="K61" t="b">
+      <c r="K61" s="1" t="b">
         <f t="array" ref="K61">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
         <v>0</v>
       </c>
@@ -3790,12 +3853,12 @@
       </c>
       <c r="Q61" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "weak": {},</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "shining": {},</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="G62">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -3839,12 +3902,12 @@
       </c>
       <c r="Q62" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "wise": {},</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "shy": {},</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="G63">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
@@ -3888,30 +3951,30 @@
       </c>
       <c r="Q63" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "witty": {},</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "skillful": {},</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="G64">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
         <v>0</v>
       </c>
-      <c r="H64" s="1">
+      <c r="H64">
         <f t="array" ref="H64">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
         <v>1</v>
       </c>
-      <c r="I64" s="1" t="str">
-        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00000</v>
-      </c>
-      <c r="J64" s="1">
+      <c r="I64" t="str">
+        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
+        <v>00000</v>
+      </c>
+      <c r="J64">
         <f t="array" ref="J64">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
         <v>59</v>
       </c>
-      <c r="K64" s="1" t="b">
+      <c r="K64" t="b">
         <f t="array" ref="K64">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
         <v>0</v>
       </c>
@@ -3937,28 +4000,16 @@
       </c>
       <c r="Q64" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "wizard": {},</v>
+        <v xml:space="preserve">    "sly": {},</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>7</v>
-      </c>
-      <c r="C65">
-        <v>-3</v>
-      </c>
-      <c r="D65">
-        <v>5</v>
-      </c>
-      <c r="E65">
-        <v>2</v>
-      </c>
-      <c r="F65">
-        <v>-3</v>
+        <v>55</v>
       </c>
       <c r="G65">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H65">
         <f t="array" ref="H65">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -3966,15 +4017,15 @@
       </c>
       <c r="I65" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>0-352-3</v>
+        <v>00000</v>
       </c>
       <c r="J65">
         <f t="array" ref="J65">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="K65" t="b">
         <f t="array" ref="K65">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L65" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
@@ -3982,41 +4033,32 @@
       </c>
       <c r="M65" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
-        <v xml:space="preserve">"enthusiasm": -3, </v>
+        <v/>
       </c>
       <c r="N65" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v xml:space="preserve">"stability": 5, </v>
+        <v/>
       </c>
       <c r="O65" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
-        <v xml:space="preserve">"insight": 2, </v>
+        <v/>
       </c>
       <c r="P65" t="str">
         <f>IF(Table1[[#This Row],[Mysticism]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Mysticism]]) &amp; """: " &amp; Table1[[#This Row],[Mysticism]] &amp; ", ")</f>
-        <v xml:space="preserve">"mysticism": -3, </v>
+        <v/>
       </c>
       <c r="Q65" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "serious": {"enthusiasm": -3, "stability": 5, "insight": 2, "mysticism": -3, },</v>
+        <v xml:space="preserve">    "strict": {},</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>26</v>
-      </c>
-      <c r="C66">
-        <v>4</v>
-      </c>
-      <c r="D66">
-        <v>-4</v>
-      </c>
-      <c r="F66">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G66">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H66">
         <f t="array" ref="H66">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -4024,15 +4066,15 @@
       </c>
       <c r="I66" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>04-402</v>
+        <v>00000</v>
       </c>
       <c r="J66">
         <f t="array" ref="J66">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="K66" t="b">
         <f t="array" ref="K66">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L66" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
@@ -4040,11 +4082,11 @@
       </c>
       <c r="M66" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
-        <v xml:space="preserve">"enthusiasm": 4, </v>
+        <v/>
       </c>
       <c r="N66" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v xml:space="preserve">"stability": -4, </v>
+        <v/>
       </c>
       <c r="O66" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
@@ -4052,42 +4094,36 @@
       </c>
       <c r="P66" t="str">
         <f>IF(Table1[[#This Row],[Mysticism]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Mysticism]]) &amp; """: " &amp; Table1[[#This Row],[Mysticism]] &amp; ", ")</f>
-        <v xml:space="preserve">"mysticism": 2, </v>
+        <v/>
       </c>
       <c r="Q66" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "adventurous": {"enthusiasm": 4, "stability": -4, "mysticism": 2, },</v>
+        <v xml:space="preserve">    "stubborn": {},</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>52</v>
-      </c>
-      <c r="C67">
-        <v>-4</v>
-      </c>
-      <c r="D67">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="G67">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H67">
         <f t="array" ref="H67">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I67" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>0-4600</v>
+        <v>00000</v>
       </c>
       <c r="J67">
         <f t="array" ref="J67">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="K67" t="b">
         <f t="array" ref="K67">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L67" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
@@ -4095,11 +4131,11 @@
       </c>
       <c r="M67" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
-        <v xml:space="preserve">"enthusiasm": -4, </v>
+        <v/>
       </c>
       <c r="N67" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v xml:space="preserve">"stability": 6, </v>
+        <v/>
       </c>
       <c r="O67" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
@@ -4111,45 +4147,36 @@
       </c>
       <c r="Q67" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "calm": {"enthusiasm": -4, "stability": 6, },</v>
+        <v xml:space="preserve">    "studious": {},</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>29</v>
-      </c>
-      <c r="B68">
+        <v>22</v>
+      </c>
+      <c r="G68">
+        <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
+        <v>0</v>
+      </c>
+      <c r="H68" s="1">
+        <f t="array" ref="H68">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
         <v>2</v>
       </c>
-      <c r="E68">
-        <v>-2</v>
-      </c>
-      <c r="F68">
-        <v>2</v>
-      </c>
-      <c r="G68">
-        <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>2</v>
-      </c>
-      <c r="H68">
-        <f t="array" ref="H68">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
-        <v>1</v>
-      </c>
-      <c r="I68" t="str">
-        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>200-22</v>
-      </c>
-      <c r="J68">
+      <c r="I68" s="1" t="str">
+        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
+        <v>00000</v>
+      </c>
+      <c r="J68" s="1">
         <f t="array" ref="J68">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>1</v>
-      </c>
-      <c r="K68" t="b">
+        <v>59</v>
+      </c>
+      <c r="K68" s="1" t="b">
         <f t="array" ref="K68">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L68" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
-        <v xml:space="preserve">"determination": 2, </v>
+        <v/>
       </c>
       <c r="M68" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
@@ -4161,36 +4188,24 @@
       </c>
       <c r="O68" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
-        <v xml:space="preserve">"insight": -2, </v>
+        <v/>
       </c>
       <c r="P68" t="str">
         <f>IF(Table1[[#This Row],[Mysticism]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Mysticism]]) &amp; """: " &amp; Table1[[#This Row],[Mysticism]] &amp; ", ")</f>
-        <v xml:space="preserve">"mysticism": 2, </v>
+        <v/>
       </c>
       <c r="Q68" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "charming": {"determination": 2, "insight": -2, "mysticism": 2, },</v>
+        <v xml:space="preserve">    "studious": {},</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>28</v>
-      </c>
-      <c r="B69">
-        <v>2</v>
-      </c>
-      <c r="D69">
-        <v>2</v>
-      </c>
-      <c r="E69">
-        <v>-4</v>
-      </c>
-      <c r="F69">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="G69">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H69">
         <f t="array" ref="H69">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -4198,19 +4213,19 @@
       </c>
       <c r="I69" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>202-42</v>
+        <v>00000</v>
       </c>
       <c r="J69">
         <f t="array" ref="J69">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="K69" t="b">
         <f t="array" ref="K69">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L69" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
-        <v xml:space="preserve">"determination": 2, </v>
+        <v/>
       </c>
       <c r="M69" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
@@ -4218,37 +4233,28 @@
       </c>
       <c r="N69" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v xml:space="preserve">"stability": 2, </v>
+        <v/>
       </c>
       <c r="O69" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
-        <v xml:space="preserve">"insight": -4, </v>
+        <v/>
       </c>
       <c r="P69" t="str">
         <f>IF(Table1[[#This Row],[Mysticism]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Mysticism]]) &amp; """: " &amp; Table1[[#This Row],[Mysticism]] &amp; ", ")</f>
-        <v xml:space="preserve">"mysticism": 2, </v>
+        <v/>
       </c>
       <c r="Q69" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "daring": {"determination": 2, "stability": 2, "insight": -4, "mysticism": 2, },</v>
+        <v xml:space="preserve">    "talented": {},</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>50</v>
-      </c>
-      <c r="B70">
-        <v>6</v>
-      </c>
-      <c r="C70">
-        <v>-2</v>
-      </c>
-      <c r="F70">
-        <v>-2</v>
+        <v>64</v>
       </c>
       <c r="G70">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H70">
         <f t="array" ref="H70">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -4256,23 +4262,23 @@
       </c>
       <c r="I70" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>6-200-2</v>
+        <v>00000</v>
       </c>
       <c r="J70">
         <f t="array" ref="J70">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="K70" t="b">
         <f t="array" ref="K70">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L70" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
-        <v xml:space="preserve">"determination": 6, </v>
+        <v/>
       </c>
       <c r="M70" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
-        <v xml:space="preserve">"enthusiasm": -2, </v>
+        <v/>
       </c>
       <c r="N70" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
@@ -4284,32 +4290,20 @@
       </c>
       <c r="P70" t="str">
         <f>IF(Table1[[#This Row],[Mysticism]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Mysticism]]) &amp; """: " &amp; Table1[[#This Row],[Mysticism]] &amp; ", ")</f>
-        <v xml:space="preserve">"mysticism": -2, </v>
+        <v/>
       </c>
       <c r="Q70" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "determined": {"determination": 6, "enthusiasm": -2, "mysticism": -2, },</v>
+        <v xml:space="preserve">    "thoughtful": {},</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>33</v>
-      </c>
-      <c r="C71">
-        <v>-4</v>
-      </c>
-      <c r="D71">
-        <v>4</v>
-      </c>
-      <c r="E71">
-        <v>6</v>
-      </c>
-      <c r="F71">
-        <v>-3</v>
+        <v>72</v>
       </c>
       <c r="G71">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H71">
         <f t="array" ref="H71">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -4317,15 +4311,15 @@
       </c>
       <c r="I71" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>0-446-3</v>
+        <v>00000</v>
       </c>
       <c r="J71">
         <f t="array" ref="J71">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="K71" t="b">
         <f t="array" ref="K71">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L71" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
@@ -4333,69 +4327,60 @@
       </c>
       <c r="M71" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
-        <v xml:space="preserve">"enthusiasm": -4, </v>
+        <v/>
       </c>
       <c r="N71" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v xml:space="preserve">"stability": 4, </v>
+        <v/>
       </c>
       <c r="O71" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
-        <v xml:space="preserve">"insight": 6, </v>
+        <v/>
       </c>
       <c r="P71" t="str">
         <f>IF(Table1[[#This Row],[Mysticism]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Mysticism]]) &amp; """: " &amp; Table1[[#This Row],[Mysticism]] &amp; ", ")</f>
-        <v xml:space="preserve">"mysticism": -3, </v>
+        <v/>
       </c>
       <c r="Q71" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "cautious": {"enthusiasm": -4, "stability": 4, "insight": 6, "mysticism": -3, },</v>
+        <v xml:space="preserve">    "timid": {},</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>5</v>
-      </c>
-      <c r="B72">
-        <v>-2</v>
-      </c>
-      <c r="C72">
-        <v>-1</v>
-      </c>
-      <c r="D72">
-        <v>6</v>
+        <v>86</v>
       </c>
       <c r="G72">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>3</v>
-      </c>
-      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="H72" s="1">
         <f t="array" ref="H72">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
         <v>1</v>
       </c>
-      <c r="I72" t="str">
-        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>-2-1600</v>
-      </c>
-      <c r="J72">
+      <c r="I72" s="1" t="str">
+        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
+        <v>00000</v>
+      </c>
+      <c r="J72" s="1">
         <f t="array" ref="J72">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>1</v>
-      </c>
-      <c r="K72" t="b">
+        <v>59</v>
+      </c>
+      <c r="K72" s="1" t="b">
         <f t="array" ref="K72">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L72" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
-        <v xml:space="preserve">"determination": -2, </v>
+        <v/>
       </c>
       <c r="M72" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
-        <v xml:space="preserve">"enthusiasm": -1, </v>
+        <v/>
       </c>
       <c r="N72" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v xml:space="preserve">"stability": 6, </v>
+        <v/>
       </c>
       <c r="O72" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
@@ -4407,22 +4392,16 @@
       </c>
       <c r="Q72" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "humble": {"determination": -2, "enthusiasm": -1, "stability": 6, },</v>
+        <v xml:space="preserve">    "tired": {},</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>51</v>
-      </c>
-      <c r="C73">
-        <v>6</v>
-      </c>
-      <c r="D73">
-        <v>-2</v>
+        <v>65</v>
       </c>
       <c r="G73">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H73">
         <f t="array" ref="H73">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -4430,15 +4409,15 @@
       </c>
       <c r="I73" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>06-200</v>
+        <v>00000</v>
       </c>
       <c r="J73">
         <f t="array" ref="J73">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="K73" t="b">
         <f t="array" ref="K73">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L73" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
@@ -4446,11 +4425,11 @@
       </c>
       <c r="M73" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
-        <v xml:space="preserve">"enthusiasm": 6, </v>
+        <v/>
       </c>
       <c r="N73" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v xml:space="preserve">"stability": -2, </v>
+        <v/>
       </c>
       <c r="O73" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
@@ -4462,25 +4441,16 @@
       </c>
       <c r="Q73" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "energetic": {"enthusiasm": 6, "stability": -2, },</v>
+        <v xml:space="preserve">    "tolerant": {},</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>42</v>
-      </c>
-      <c r="B74">
-        <v>-2</v>
-      </c>
-      <c r="C74">
-        <v>4</v>
-      </c>
-      <c r="D74">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="G74">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H74">
         <f t="array" ref="H74">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -4488,27 +4458,27 @@
       </c>
       <c r="I74" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>-24200</v>
+        <v>00000</v>
       </c>
       <c r="J74">
         <f t="array" ref="J74">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="K74" t="b">
         <f t="array" ref="K74">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L74" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
-        <v xml:space="preserve">"determination": -2, </v>
+        <v/>
       </c>
       <c r="M74" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
-        <v xml:space="preserve">"enthusiasm": 4, </v>
+        <v/>
       </c>
       <c r="N74" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v xml:space="preserve">"stability": 2, </v>
+        <v/>
       </c>
       <c r="O74" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
@@ -4520,25 +4490,16 @@
       </c>
       <c r="Q74" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "hopeful": {"determination": -2, "enthusiasm": 4, "stability": 2, },</v>
+        <v xml:space="preserve">    "trustworthy": {},</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>45</v>
-      </c>
-      <c r="B75">
-        <v>4</v>
-      </c>
-      <c r="C75">
-        <v>-3</v>
-      </c>
-      <c r="E75">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="G75">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H75">
         <f t="array" ref="H75">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -4546,23 +4507,23 @@
       </c>
       <c r="I75" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>4-3040</v>
+        <v>00000</v>
       </c>
       <c r="J75">
         <f t="array" ref="J75">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="K75" t="b">
         <f t="array" ref="K75">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L75" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
-        <v xml:space="preserve">"determination": 4, </v>
+        <v/>
       </c>
       <c r="M75" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
-        <v xml:space="preserve">"enthusiasm": -3, </v>
+        <v/>
       </c>
       <c r="N75" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
@@ -4570,7 +4531,7 @@
       </c>
       <c r="O75" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
-        <v xml:space="preserve">"insight": 4, </v>
+        <v/>
       </c>
       <c r="P75" t="str">
         <f>IF(Table1[[#This Row],[Mysticism]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Mysticism]]) &amp; """: " &amp; Table1[[#This Row],[Mysticism]] &amp; ", ")</f>
@@ -4578,25 +4539,16 @@
       </c>
       <c r="Q75" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "ambitious": {"determination": 4, "enthusiasm": -3, "insight": 4, },</v>
+        <v xml:space="preserve">    "weak": {},</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>6</v>
-      </c>
-      <c r="B76">
-        <v>5</v>
-      </c>
-      <c r="C76">
-        <v>2</v>
-      </c>
-      <c r="E76">
-        <v>-2</v>
+        <v>68</v>
       </c>
       <c r="G76">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H76">
         <f t="array" ref="H76">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -4604,23 +4556,23 @@
       </c>
       <c r="I76" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>520-20</v>
+        <v>00000</v>
       </c>
       <c r="J76">
         <f t="array" ref="J76">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="K76" t="b">
         <f t="array" ref="K76">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L76" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
-        <v xml:space="preserve">"determination": 5, </v>
+        <v/>
       </c>
       <c r="M76" t="str">
         <f>IF(Table1[[#This Row],[Enthusiasm]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Enthusiasm]]) &amp; """: " &amp; Table1[[#This Row],[Enthusiasm]] &amp; ", ")</f>
-        <v xml:space="preserve">"enthusiasm": 2, </v>
+        <v/>
       </c>
       <c r="N76" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
@@ -4628,7 +4580,7 @@
       </c>
       <c r="O76" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
-        <v xml:space="preserve">"insight": -2, </v>
+        <v/>
       </c>
       <c r="P76" t="str">
         <f>IF(Table1[[#This Row],[Mysticism]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Mysticism]]) &amp; """: " &amp; Table1[[#This Row],[Mysticism]] &amp; ", ")</f>
@@ -4636,25 +4588,16 @@
       </c>
       <c r="Q76" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "brave": {"determination": 5, "enthusiasm": 2, "insight": -2, },</v>
+        <v xml:space="preserve">    "wise": {},</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>18</v>
-      </c>
-      <c r="D77">
-        <v>-2</v>
-      </c>
-      <c r="E77">
-        <v>6</v>
-      </c>
-      <c r="F77">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="G77">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H77">
         <f t="array" ref="H77">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
@@ -4662,15 +4605,15 @@
       </c>
       <c r="I77" t="str">
         <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00-262</v>
+        <v>00000</v>
       </c>
       <c r="J77">
         <f t="array" ref="J77">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="K77" t="b">
         <f t="array" ref="K77">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L77" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
@@ -4682,53 +4625,44 @@
       </c>
       <c r="N77" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v xml:space="preserve">"stability": -2, </v>
+        <v/>
       </c>
       <c r="O77" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
-        <v xml:space="preserve">"insight": 6, </v>
+        <v/>
       </c>
       <c r="P77" t="str">
         <f>IF(Table1[[#This Row],[Mysticism]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Mysticism]]) &amp; """: " &amp; Table1[[#This Row],[Mysticism]] &amp; ", ")</f>
-        <v xml:space="preserve">"mysticism": 2, </v>
+        <v/>
       </c>
       <c r="Q77" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "brilliant": {"stability": -2, "insight": 6, "mysticism": 2, },</v>
+        <v xml:space="preserve">    "witty": {},</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>19</v>
-      </c>
-      <c r="D78">
-        <v>-2</v>
-      </c>
-      <c r="E78">
-        <v>2</v>
-      </c>
-      <c r="F78">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="G78">
         <f>SUM(Table1[[#This Row],[Determination]:[Mysticism]])</f>
-        <v>6</v>
-      </c>
-      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="H78" s="1">
         <f t="array" ref="H78">SUM(IF(Table1[Name]=Table1[[#This Row],[Name]],1,0))</f>
         <v>1</v>
       </c>
-      <c r="I78" t="str">
-        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
-        <v>00-226</v>
-      </c>
-      <c r="J78">
+      <c r="I78" s="1" t="str">
+        <f>CONCATENATE(IF(Table1[[#This Row],[Determination]]=0,"0",Table1[[#This Row],[Determination]]),IF(Table1[[#This Row],[Enthusiasm]]=0,"0",Table1[[#This Row],[Enthusiasm]]),IF(Table1[[#This Row],[Stability]]=0,"0",Table1[[#This Row],[Stability]]),IF(Table1[[#This Row],[Insight]]=0,"0",Table1[[#This Row],[Insight]]),IF(Table1[[#This Row],[Mysticism]]=0,"0",Table1[[#This Row],[Mysticism]]))</f>
+        <v>00000</v>
+      </c>
+      <c r="J78" s="1">
         <f t="array" ref="J78">SUM(IF(Table1[string values]=Table1[[#This Row],[string values]],1,0))</f>
-        <v>1</v>
-      </c>
-      <c r="K78" t="b">
+        <v>59</v>
+      </c>
+      <c r="K78" s="1" t="b">
         <f t="array" ref="K78">IF(Table1[[#This Row],[Name]]=0, "", AND(Table1[[#This Row],[unique name]]=1, Table1[[#This Row],[unique values]]=1))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L78" t="str">
         <f>IF(Table1[[#This Row],[Determination]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Determination]]) &amp; """: " &amp; Table1[[#This Row],[Determination]] &amp; ", ")</f>
@@ -4740,24 +4674,24 @@
       </c>
       <c r="N78" t="str">
         <f>IF(Table1[[#This Row],[Stability]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Stability]]) &amp; """: " &amp; Table1[[#This Row],[Stability]] &amp; ", ")</f>
-        <v xml:space="preserve">"stability": -2, </v>
+        <v/>
       </c>
       <c r="O78" t="str">
         <f>IF(Table1[[#This Row],[Insight]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Insight]]) &amp; """: " &amp; Table1[[#This Row],[Insight]] &amp; ", ")</f>
-        <v xml:space="preserve">"insight": 2, </v>
+        <v/>
       </c>
       <c r="P78" t="str">
         <f>IF(Table1[[#This Row],[Mysticism]]=0, "", """" &amp; LOWER(Table1[[#Headers],[Mysticism]]) &amp; """: " &amp; Table1[[#This Row],[Mysticism]] &amp; ", ")</f>
-        <v xml:space="preserve">"mysticism": 6, </v>
+        <v/>
       </c>
       <c r="Q78" t="str">
         <f>CONCATENATE("    ", """", Table1[[#This Row],[Name]], """: {", Table1[[#This Row],[Column1]], Table1[[#This Row],[Column2]], Table1[[#This Row],[Column3]], Table1[[#This Row],[Column4]], Table1[[#This Row],[Column5]], "},")</f>
-        <v xml:space="preserve">    "creative": {"stability": -2, "insight": 2, "mysticism": 6, },</v>
+        <v xml:space="preserve">    "wizard": {},</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K3:K78">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>